<commit_message>
Updated the schema for string enum values
</commit_message>
<xml_diff>
--- a/CancerSummary/SchemaUpdates.xlsx
+++ b/CancerSummary/SchemaUpdates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>SOURCE</t>
   </si>
@@ -45,12 +45,6 @@
   </si>
   <si>
     <t>Epithelium</t>
-  </si>
-  <si>
-    <t>["Serous High", "Serous Low", "Clear Cell (automatically Grade 3)", "Undifferentiated (automatically Grade 3)", "Endometroid",  "Mucinous", "Transitional", "Mixed Epithelial Types", "Endometroid,Mucinous, Clear Cell", "Mixed Endometroid, Serous", "Other", null]</t>
-  </si>
-  <si>
-    <t>["Adenocarcinoma - NOS", "Carcinosarcoma", "Endometrioid, Clear Cell", "Pseudomyxoma peritoneii", "Serous - NOS"]</t>
   </si>
   <si>
     <t>ER_STATUS</t>
@@ -145,9 +139,6 @@
     <t>meaning of "N" is not available</t>
   </si>
   <si>
-    <t>NEW_VALUES_ADDED</t>
-  </si>
-  <si>
     <t>meaning of "U" is not available</t>
   </si>
   <si>
@@ -206,6 +197,67 @@
   </si>
   <si>
     <t>Meaning of new values not available</t>
+  </si>
+  <si>
+    <t>HistoPath_BreastCancer</t>
+  </si>
+  <si>
+    <t>Malignant</t>
+  </si>
+  <si>
+    <t>Need description for enum values</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>["L", "R"]</t>
+  </si>
+  <si>
+    <t>["U"]</t>
+  </si>
+  <si>
+    <t>ScreenDetected</t>
+  </si>
+  <si>
+    <t>["Y", "N"]</t>
+  </si>
+  <si>
+    <t>["NK"]</t>
+  </si>
+  <si>
+    <t>meaning of "NK" is not available</t>
+  </si>
+  <si>
+    <t>UPDATED</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>"Carcinosarcoma", "Serous High", "Serous Low", "Clear Cell (automatically Grade 3)", 
+                "Undifferentiated (automatically Grade 3)", "Endometroid", "Mucinous", "Transitional",  "Mixed Epithelial Types", "Endometroid, Mucinous, Clear Cell", "Mixed Endometroid, Serous", "Other", null</t>
+  </si>
+  <si>
+    <t>["Adenocarcinoma - NOS",  "Endometrioid, Clear Cell", "Pseudomyxoma peritoneii", "Serous - NOS"]</t>
+  </si>
+  <si>
+    <t>NEW_VALUES</t>
+  </si>
+  <si>
+    <t>InvasiveGrade</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, null]</t>
+  </si>
+  <si>
+    <t>["NA"]</t>
+  </si>
+  <si>
+    <t>Need to know what is "NA" and convert the data accordingly</t>
   </si>
 </sst>
 </file>
@@ -243,7 +295,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -273,10 +325,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -288,10 +338,58 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -300,24 +398,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -328,91 +409,103 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -705,139 +798,233 @@
     <col min="1" max="2" width="24.54296875" customWidth="1"/>
     <col min="3" max="3" width="69.54296875" customWidth="1"/>
     <col min="4" max="4" width="66.26953125" customWidth="1"/>
-    <col min="5" max="5" width="35.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="27"/>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="144.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="27"/>
+      <c r="B5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="D5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="185.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="27"/>
+      <c r="B6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="25"/>
+      <c r="B8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="29"/>
+      <c r="B10" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="29"/>
+      <c r="B11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="144.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="185.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="8"/>
+      <c r="F11" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="26"/>
+      <c r="B12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A9:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the excel file for schema changes
</commit_message>
<xml_diff>
--- a/CancerSummary/SchemaUpdates.xlsx
+++ b/CancerSummary/SchemaUpdates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>SOURCE</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Need to know what is "NA" and convert the data accordingly</t>
+  </si>
+  <si>
+    <t>Need to know whether the new values are valid or not</t>
   </si>
 </sst>
 </file>
@@ -420,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -479,7 +482,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,6 +491,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -505,6 +510,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -790,7 +798,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,7 +826,7 @@
       <c r="E1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>36</v>
       </c>
     </row>
@@ -945,7 +953,9 @@
       <c r="D8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="30" t="s">
+        <v>46</v>
+      </c>
       <c r="F8" s="12" t="s">
         <v>38</v>
       </c>
@@ -961,26 +971,28 @@
         <v>28</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="E9" s="21"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="29"/>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="23" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="29"/>
@@ -993,7 +1005,7 @@
       <c r="D11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="20" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="12" t="s">
@@ -1011,7 +1023,7 @@
       <c r="D12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>35</v>
       </c>
       <c r="F12" s="12" t="s">

</xml_diff>

<commit_message>
Updates to schema variables and scripts
Updated the schemas after confirming the differences in variables and enum values. Updated the scripts to handle the changes in the schema and clean the data
</commit_message>
<xml_diff>
--- a/CancerSummary/SchemaUpdates.xlsx
+++ b/CancerSummary/SchemaUpdates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>SOURCE</t>
   </si>
@@ -136,9 +136,6 @@
     <t>COMMENTS</t>
   </si>
   <si>
-    <t>meaning of "N" is not available</t>
-  </si>
-  <si>
     <t>meaning of "U" is not available</t>
   </si>
   <si>
@@ -226,22 +223,12 @@
     <t>["NK"]</t>
   </si>
   <si>
-    <t>meaning of "NK" is not available</t>
-  </si>
-  <si>
     <t>UPDATED</t>
   </si>
   <si>
     <t>YES</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>"Carcinosarcoma", "Serous High", "Serous Low", "Clear Cell (automatically Grade 3)", 
-                "Undifferentiated (automatically Grade 3)", "Endometroid", "Mucinous", "Transitional",  "Mixed Epithelial Types", "Endometroid, Mucinous, Clear Cell", "Mixed Endometroid, Serous", "Other", null</t>
-  </si>
-  <si>
     <t>["Adenocarcinoma - NOS",  "Endometrioid, Clear Cell", "Pseudomyxoma peritoneii", "Serous - NOS"]</t>
   </si>
   <si>
@@ -257,10 +244,26 @@
     <t>["NA"]</t>
   </si>
   <si>
-    <t>Need to know what is "NA" and convert the data accordingly</t>
-  </si>
-  <si>
-    <t>Need to know whether the new values are valid or not</t>
+    <t>["Carcinosarcoma", "Serous High", "Serous Low", "Clear Cell (automatically Grade 3)", 
+                "Undifferentiated (automatically Grade 3)", "Endometroid", "Mucinous", "Transitional",  "Mixed Epithelial Types", "Endometroid, Mucinous, Clear Cell", "Mixed Endometroid, Serous", "Other", null]</t>
+  </si>
+  <si>
+    <t>U: Unknown</t>
+  </si>
+  <si>
+    <t>NK: Not Known</t>
+  </si>
+  <si>
+    <t>All are valid values and can be added</t>
+  </si>
+  <si>
+    <t>Added the description</t>
+  </si>
+  <si>
+    <t>"N" is Not reported and is same as null. Need to covert all null to N in the data</t>
+  </si>
+  <si>
+    <t>"NA" means Not assessable</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -470,50 +473,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -797,16 +803,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="24.54296875" customWidth="1"/>
-    <col min="3" max="3" width="69.54296875" customWidth="1"/>
-    <col min="4" max="4" width="66.26953125" customWidth="1"/>
-    <col min="5" max="5" width="51.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.81640625" customWidth="1"/>
+    <col min="4" max="4" width="40.26953125" customWidth="1"/>
+    <col min="5" max="5" width="29.81640625" style="31" customWidth="1"/>
     <col min="6" max="6" width="8.7265625" style="13"/>
   </cols>
   <sheetData>
@@ -821,17 +827,17 @@
         <v>1</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>36</v>
+      <c r="F1" s="16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="70" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -843,15 +849,15 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>17</v>
+      <c r="E2" s="26" t="s">
+        <v>16</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -861,15 +867,15 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>17</v>
+      <c r="E3" s="27" t="s">
+        <v>16</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
@@ -879,51 +885,51 @@
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="144.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="22"/>
+      <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="144.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="F5" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="185.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="22"/>
+      <c r="B6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="185.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
-      <c r="B6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="E6" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>25</v>
-      </c>
       <c r="F6" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -935,99 +941,101 @@
       <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>16</v>
+      <c r="E7" s="26" t="s">
+        <v>46</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="25"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A8" s="20"/>
       <c r="B8" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="24"/>
+      <c r="B10" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D10" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="E10" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="24"/>
+      <c r="B11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
-      <c r="B10" s="22" t="s">
+      <c r="C11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="F11" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="21"/>
+      <c r="B12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="29"/>
-      <c r="B11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="26"/>
-      <c r="B12" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="20" t="s">
+      <c r="F12" s="18" t="s">
         <v>35</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>